<commit_message>
ACTUALIZACION DEL PERFIL DE PROYECTO
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/ELICITACION/1.2 CRONOGRAMA/G8_CRONOGRAMA_V3.0.xlsx
+++ b/DOCUMENTACION/ELICITACION/1.2 CRONOGRAMA/G8_CRONOGRAMA_V3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Desktop\FUNDAMENTOS\AlfonsoArroyo_14538_Grupo8_FINGSW\DOCUMENTACION\ELICITACION\1.2 CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B09853-8535-45F6-9E57-F745947F5C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F18831-ADC4-4463-B4E3-C262FCA31AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{AB7E0F87-5473-4D2E-88B4-002DBDAD9EEB}"/>
   </bookViews>
@@ -666,6 +666,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,24 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -723,6 +720,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,14 +735,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D665D8-8001-4FBD-9099-1C04366A38F2}">
   <dimension ref="B1:EE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW48" sqref="AW48"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ9" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1097,25 +1097,25 @@
   <sheetData>
     <row r="1" spans="2:135" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:135" x14ac:dyDescent="0.25">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="52"/>
+      <c r="C2" s="51"/>
     </row>
     <row r="3" spans="2:135" x14ac:dyDescent="0.25">
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="4" spans="2:135" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="2:135" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
@@ -1127,307 +1127,307 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:135" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="54"/>
-      <c r="C9" s="56">
+      <c r="B9" s="53"/>
+      <c r="C9" s="55">
         <v>45433</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:135" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="48"/>
-      <c r="Z10" s="48"/>
-      <c r="AA10" s="48"/>
-      <c r="AB10" s="48"/>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="48"/>
-      <c r="AE10" s="48"/>
-      <c r="AF10" s="48"/>
-      <c r="AG10" s="48"/>
-      <c r="AH10" s="48"/>
-      <c r="AI10" s="48"/>
-      <c r="AJ10" s="48"/>
-      <c r="AK10" s="48"/>
-      <c r="AL10" s="48"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="57"/>
+      <c r="AC10" s="57"/>
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="57"/>
+      <c r="AI10" s="57"/>
+      <c r="AJ10" s="57"/>
+      <c r="AK10" s="57"/>
+      <c r="AL10" s="57"/>
       <c r="AM10" s="58"/>
-      <c r="AN10" s="46" t="s">
+      <c r="AN10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="AO10" s="46"/>
-      <c r="AP10" s="46"/>
-      <c r="AQ10" s="46"/>
-      <c r="AR10" s="46"/>
-      <c r="AS10" s="46"/>
-      <c r="AT10" s="46"/>
-      <c r="AU10" s="46"/>
-      <c r="AV10" s="46"/>
-      <c r="AW10" s="46"/>
-      <c r="AX10" s="46"/>
-      <c r="AY10" s="46"/>
-      <c r="AZ10" s="46"/>
-      <c r="BA10" s="46"/>
-      <c r="BB10" s="46"/>
-      <c r="BC10" s="46"/>
-      <c r="BD10" s="46"/>
-      <c r="BE10" s="46"/>
-      <c r="BF10" s="46"/>
-      <c r="BG10" s="46"/>
-      <c r="BH10" s="46"/>
-      <c r="BI10" s="46"/>
-      <c r="BJ10" s="46"/>
-      <c r="BK10" s="46"/>
-      <c r="BL10" s="46"/>
-      <c r="BM10" s="46"/>
-      <c r="BN10" s="46"/>
-      <c r="BO10" s="46"/>
-      <c r="BP10" s="46"/>
-      <c r="BQ10" s="47"/>
-      <c r="BR10" s="46" t="s">
+      <c r="AO10" s="42"/>
+      <c r="AP10" s="42"/>
+      <c r="AQ10" s="42"/>
+      <c r="AR10" s="42"/>
+      <c r="AS10" s="42"/>
+      <c r="AT10" s="42"/>
+      <c r="AU10" s="42"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="42"/>
+      <c r="AX10" s="42"/>
+      <c r="AY10" s="42"/>
+      <c r="AZ10" s="42"/>
+      <c r="BA10" s="42"/>
+      <c r="BB10" s="42"/>
+      <c r="BC10" s="42"/>
+      <c r="BD10" s="42"/>
+      <c r="BE10" s="42"/>
+      <c r="BF10" s="42"/>
+      <c r="BG10" s="42"/>
+      <c r="BH10" s="42"/>
+      <c r="BI10" s="42"/>
+      <c r="BJ10" s="42"/>
+      <c r="BK10" s="42"/>
+      <c r="BL10" s="42"/>
+      <c r="BM10" s="42"/>
+      <c r="BN10" s="42"/>
+      <c r="BO10" s="42"/>
+      <c r="BP10" s="42"/>
+      <c r="BQ10" s="43"/>
+      <c r="BR10" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="BS10" s="46"/>
-      <c r="BT10" s="46"/>
-      <c r="BU10" s="46"/>
-      <c r="BV10" s="46"/>
-      <c r="BW10" s="46"/>
-      <c r="BX10" s="46"/>
-      <c r="BY10" s="46"/>
-      <c r="BZ10" s="46"/>
-      <c r="CA10" s="46"/>
-      <c r="CB10" s="46"/>
-      <c r="CC10" s="46"/>
-      <c r="CD10" s="46"/>
-      <c r="CE10" s="46"/>
-      <c r="CF10" s="46"/>
-      <c r="CG10" s="46"/>
-      <c r="CH10" s="46"/>
-      <c r="CI10" s="46"/>
-      <c r="CJ10" s="46"/>
-      <c r="CK10" s="46"/>
-      <c r="CL10" s="46"/>
-      <c r="CM10" s="46"/>
-      <c r="CN10" s="46"/>
-      <c r="CO10" s="46"/>
-      <c r="CP10" s="46"/>
-      <c r="CQ10" s="46"/>
-      <c r="CR10" s="46"/>
-      <c r="CS10" s="46"/>
-      <c r="CT10" s="46"/>
-      <c r="CU10" s="46"/>
-      <c r="CV10" s="47"/>
-      <c r="CW10" s="48" t="s">
+      <c r="BS10" s="42"/>
+      <c r="BT10" s="42"/>
+      <c r="BU10" s="42"/>
+      <c r="BV10" s="42"/>
+      <c r="BW10" s="42"/>
+      <c r="BX10" s="42"/>
+      <c r="BY10" s="42"/>
+      <c r="BZ10" s="42"/>
+      <c r="CA10" s="42"/>
+      <c r="CB10" s="42"/>
+      <c r="CC10" s="42"/>
+      <c r="CD10" s="42"/>
+      <c r="CE10" s="42"/>
+      <c r="CF10" s="42"/>
+      <c r="CG10" s="42"/>
+      <c r="CH10" s="42"/>
+      <c r="CI10" s="42"/>
+      <c r="CJ10" s="42"/>
+      <c r="CK10" s="42"/>
+      <c r="CL10" s="42"/>
+      <c r="CM10" s="42"/>
+      <c r="CN10" s="42"/>
+      <c r="CO10" s="42"/>
+      <c r="CP10" s="42"/>
+      <c r="CQ10" s="42"/>
+      <c r="CR10" s="42"/>
+      <c r="CS10" s="42"/>
+      <c r="CT10" s="42"/>
+      <c r="CU10" s="42"/>
+      <c r="CV10" s="43"/>
+      <c r="CW10" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="CX10" s="48"/>
-      <c r="CY10" s="48"/>
-      <c r="CZ10" s="48"/>
-      <c r="DA10" s="48"/>
-      <c r="DB10" s="48"/>
-      <c r="DC10" s="48"/>
-      <c r="DD10" s="48"/>
-      <c r="DE10" s="48"/>
-      <c r="DF10" s="48"/>
-      <c r="DG10" s="48"/>
-      <c r="DH10" s="48"/>
-      <c r="DI10" s="48"/>
-      <c r="DJ10" s="48"/>
-      <c r="DK10" s="48"/>
-      <c r="DL10" s="48"/>
-      <c r="DM10" s="48"/>
-      <c r="DN10" s="48"/>
-      <c r="DO10" s="48"/>
-      <c r="DP10" s="48"/>
-      <c r="DQ10" s="48"/>
-      <c r="DR10" s="48"/>
-      <c r="DS10" s="48"/>
-      <c r="DT10" s="48"/>
-      <c r="DU10" s="48"/>
-      <c r="DV10" s="48"/>
-      <c r="DW10" s="48"/>
-      <c r="DX10" s="48"/>
-      <c r="DY10" s="48"/>
-      <c r="DZ10" s="48"/>
-      <c r="EA10" s="48"/>
+      <c r="CX10" s="57"/>
+      <c r="CY10" s="57"/>
+      <c r="CZ10" s="57"/>
+      <c r="DA10" s="57"/>
+      <c r="DB10" s="57"/>
+      <c r="DC10" s="57"/>
+      <c r="DD10" s="57"/>
+      <c r="DE10" s="57"/>
+      <c r="DF10" s="57"/>
+      <c r="DG10" s="57"/>
+      <c r="DH10" s="57"/>
+      <c r="DI10" s="57"/>
+      <c r="DJ10" s="57"/>
+      <c r="DK10" s="57"/>
+      <c r="DL10" s="57"/>
+      <c r="DM10" s="57"/>
+      <c r="DN10" s="57"/>
+      <c r="DO10" s="57"/>
+      <c r="DP10" s="57"/>
+      <c r="DQ10" s="57"/>
+      <c r="DR10" s="57"/>
+      <c r="DS10" s="57"/>
+      <c r="DT10" s="57"/>
+      <c r="DU10" s="57"/>
+      <c r="DV10" s="57"/>
+      <c r="DW10" s="57"/>
+      <c r="DX10" s="57"/>
+      <c r="DY10" s="57"/>
+      <c r="DZ10" s="57"/>
+      <c r="EA10" s="57"/>
     </row>
     <row r="11" spans="2:135" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="48"/>
-      <c r="AE11" s="48"/>
-      <c r="AF11" s="48"/>
-      <c r="AG11" s="48"/>
-      <c r="AH11" s="48"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="57"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="57"/>
+      <c r="AC11" s="57"/>
+      <c r="AD11" s="57"/>
+      <c r="AE11" s="57"/>
+      <c r="AF11" s="57"/>
+      <c r="AG11" s="57"/>
+      <c r="AH11" s="57"/>
       <c r="AI11" s="59"/>
       <c r="AJ11" s="59"/>
       <c r="AK11" s="59"/>
       <c r="AL11" s="59"/>
       <c r="AM11" s="60"/>
-      <c r="AN11" s="46"/>
-      <c r="AO11" s="46"/>
-      <c r="AP11" s="46"/>
-      <c r="AQ11" s="46"/>
-      <c r="AR11" s="46"/>
-      <c r="AS11" s="46"/>
-      <c r="AT11" s="46"/>
-      <c r="AU11" s="46"/>
-      <c r="AV11" s="46"/>
-      <c r="AW11" s="46"/>
-      <c r="AX11" s="46"/>
-      <c r="AY11" s="46"/>
-      <c r="AZ11" s="46"/>
-      <c r="BA11" s="46"/>
-      <c r="BB11" s="46"/>
-      <c r="BC11" s="46"/>
-      <c r="BD11" s="46"/>
-      <c r="BE11" s="46"/>
-      <c r="BF11" s="46"/>
-      <c r="BG11" s="46"/>
-      <c r="BH11" s="46"/>
-      <c r="BI11" s="46"/>
-      <c r="BJ11" s="46"/>
-      <c r="BK11" s="46"/>
-      <c r="BL11" s="46"/>
-      <c r="BM11" s="46"/>
-      <c r="BN11" s="46"/>
-      <c r="BO11" s="46"/>
-      <c r="BP11" s="46"/>
-      <c r="BQ11" s="47"/>
-      <c r="BR11" s="46"/>
-      <c r="BS11" s="46"/>
-      <c r="BT11" s="46"/>
-      <c r="BU11" s="46"/>
-      <c r="BV11" s="46"/>
-      <c r="BW11" s="46"/>
-      <c r="BX11" s="46"/>
-      <c r="BY11" s="46"/>
-      <c r="BZ11" s="46"/>
-      <c r="CA11" s="46"/>
-      <c r="CB11" s="46"/>
-      <c r="CC11" s="46"/>
-      <c r="CD11" s="46"/>
-      <c r="CE11" s="46"/>
-      <c r="CF11" s="46"/>
-      <c r="CG11" s="46"/>
-      <c r="CH11" s="46"/>
-      <c r="CI11" s="46"/>
-      <c r="CJ11" s="46"/>
-      <c r="CK11" s="46"/>
-      <c r="CL11" s="46"/>
-      <c r="CM11" s="46"/>
-      <c r="CN11" s="46"/>
-      <c r="CO11" s="46"/>
-      <c r="CP11" s="46"/>
-      <c r="CQ11" s="46"/>
-      <c r="CR11" s="46"/>
-      <c r="CS11" s="46"/>
-      <c r="CT11" s="46"/>
-      <c r="CU11" s="46"/>
-      <c r="CV11" s="47"/>
-      <c r="CW11" s="48"/>
-      <c r="CX11" s="48"/>
-      <c r="CY11" s="48"/>
-      <c r="CZ11" s="48"/>
-      <c r="DA11" s="48"/>
-      <c r="DB11" s="48"/>
-      <c r="DC11" s="48"/>
-      <c r="DD11" s="48"/>
-      <c r="DE11" s="48"/>
-      <c r="DF11" s="48"/>
-      <c r="DG11" s="48"/>
-      <c r="DH11" s="48"/>
-      <c r="DI11" s="48"/>
-      <c r="DJ11" s="48"/>
-      <c r="DK11" s="48"/>
-      <c r="DL11" s="48"/>
-      <c r="DM11" s="48"/>
-      <c r="DN11" s="48"/>
-      <c r="DO11" s="48"/>
-      <c r="DP11" s="48"/>
-      <c r="DQ11" s="48"/>
-      <c r="DR11" s="48"/>
-      <c r="DS11" s="48"/>
-      <c r="DT11" s="48"/>
-      <c r="DU11" s="48"/>
-      <c r="DV11" s="48"/>
-      <c r="DW11" s="48"/>
-      <c r="DX11" s="48"/>
-      <c r="DY11" s="48"/>
-      <c r="DZ11" s="48"/>
-      <c r="EA11" s="48"/>
+      <c r="AN11" s="42"/>
+      <c r="AO11" s="42"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="42"/>
+      <c r="AR11" s="42"/>
+      <c r="AS11" s="42"/>
+      <c r="AT11" s="42"/>
+      <c r="AU11" s="42"/>
+      <c r="AV11" s="42"/>
+      <c r="AW11" s="42"/>
+      <c r="AX11" s="42"/>
+      <c r="AY11" s="42"/>
+      <c r="AZ11" s="42"/>
+      <c r="BA11" s="42"/>
+      <c r="BB11" s="42"/>
+      <c r="BC11" s="42"/>
+      <c r="BD11" s="42"/>
+      <c r="BE11" s="42"/>
+      <c r="BF11" s="42"/>
+      <c r="BG11" s="42"/>
+      <c r="BH11" s="42"/>
+      <c r="BI11" s="42"/>
+      <c r="BJ11" s="42"/>
+      <c r="BK11" s="42"/>
+      <c r="BL11" s="42"/>
+      <c r="BM11" s="42"/>
+      <c r="BN11" s="42"/>
+      <c r="BO11" s="42"/>
+      <c r="BP11" s="42"/>
+      <c r="BQ11" s="43"/>
+      <c r="BR11" s="42"/>
+      <c r="BS11" s="42"/>
+      <c r="BT11" s="42"/>
+      <c r="BU11" s="42"/>
+      <c r="BV11" s="42"/>
+      <c r="BW11" s="42"/>
+      <c r="BX11" s="42"/>
+      <c r="BY11" s="42"/>
+      <c r="BZ11" s="42"/>
+      <c r="CA11" s="42"/>
+      <c r="CB11" s="42"/>
+      <c r="CC11" s="42"/>
+      <c r="CD11" s="42"/>
+      <c r="CE11" s="42"/>
+      <c r="CF11" s="42"/>
+      <c r="CG11" s="42"/>
+      <c r="CH11" s="42"/>
+      <c r="CI11" s="42"/>
+      <c r="CJ11" s="42"/>
+      <c r="CK11" s="42"/>
+      <c r="CL11" s="42"/>
+      <c r="CM11" s="42"/>
+      <c r="CN11" s="42"/>
+      <c r="CO11" s="42"/>
+      <c r="CP11" s="42"/>
+      <c r="CQ11" s="42"/>
+      <c r="CR11" s="42"/>
+      <c r="CS11" s="42"/>
+      <c r="CT11" s="42"/>
+      <c r="CU11" s="42"/>
+      <c r="CV11" s="43"/>
+      <c r="CW11" s="57"/>
+      <c r="CX11" s="57"/>
+      <c r="CY11" s="57"/>
+      <c r="CZ11" s="57"/>
+      <c r="DA11" s="57"/>
+      <c r="DB11" s="57"/>
+      <c r="DC11" s="57"/>
+      <c r="DD11" s="57"/>
+      <c r="DE11" s="57"/>
+      <c r="DF11" s="57"/>
+      <c r="DG11" s="57"/>
+      <c r="DH11" s="57"/>
+      <c r="DI11" s="57"/>
+      <c r="DJ11" s="57"/>
+      <c r="DK11" s="57"/>
+      <c r="DL11" s="57"/>
+      <c r="DM11" s="57"/>
+      <c r="DN11" s="57"/>
+      <c r="DO11" s="57"/>
+      <c r="DP11" s="57"/>
+      <c r="DQ11" s="57"/>
+      <c r="DR11" s="57"/>
+      <c r="DS11" s="57"/>
+      <c r="DT11" s="57"/>
+      <c r="DU11" s="57"/>
+      <c r="DV11" s="57"/>
+      <c r="DW11" s="57"/>
+      <c r="DX11" s="57"/>
+      <c r="DY11" s="57"/>
+      <c r="DZ11" s="57"/>
+      <c r="EA11" s="57"/>
     </row>
     <row r="12" spans="2:135" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
@@ -1435,164 +1435,164 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="40" t="s">
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="40" t="s">
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="40" t="s">
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="46"/>
+      <c r="Z12" s="46"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="41"/>
+      <c r="AC12" s="46"/>
+      <c r="AD12" s="46"/>
+      <c r="AE12" s="46"/>
+      <c r="AF12" s="46"/>
+      <c r="AG12" s="46"/>
+      <c r="AH12" s="46"/>
       <c r="AI12" s="61"/>
       <c r="AJ12" s="61"/>
       <c r="AK12" s="61"/>
       <c r="AL12" s="61"/>
       <c r="AM12" s="61"/>
-      <c r="AN12" s="41"/>
-      <c r="AO12" s="42"/>
-      <c r="AP12" s="40" t="s">
+      <c r="AN12" s="46"/>
+      <c r="AO12" s="47"/>
+      <c r="AP12" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="AQ12" s="41"/>
-      <c r="AR12" s="41"/>
-      <c r="AS12" s="41"/>
-      <c r="AT12" s="41"/>
-      <c r="AU12" s="41"/>
-      <c r="AV12" s="42"/>
-      <c r="AW12" s="40" t="s">
+      <c r="AQ12" s="46"/>
+      <c r="AR12" s="46"/>
+      <c r="AS12" s="46"/>
+      <c r="AT12" s="46"/>
+      <c r="AU12" s="46"/>
+      <c r="AV12" s="47"/>
+      <c r="AW12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AX12" s="41"/>
-      <c r="AY12" s="41"/>
-      <c r="AZ12" s="41"/>
-      <c r="BA12" s="41"/>
-      <c r="BB12" s="41"/>
-      <c r="BC12" s="42"/>
-      <c r="BD12" s="40" t="s">
+      <c r="AX12" s="46"/>
+      <c r="AY12" s="46"/>
+      <c r="AZ12" s="46"/>
+      <c r="BA12" s="46"/>
+      <c r="BB12" s="46"/>
+      <c r="BC12" s="47"/>
+      <c r="BD12" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="BE12" s="41"/>
-      <c r="BF12" s="41"/>
-      <c r="BG12" s="41"/>
-      <c r="BH12" s="41"/>
-      <c r="BI12" s="41"/>
-      <c r="BJ12" s="42"/>
-      <c r="BK12" s="40" t="s">
+      <c r="BE12" s="46"/>
+      <c r="BF12" s="46"/>
+      <c r="BG12" s="46"/>
+      <c r="BH12" s="46"/>
+      <c r="BI12" s="46"/>
+      <c r="BJ12" s="47"/>
+      <c r="BK12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="BL12" s="41"/>
-      <c r="BM12" s="41"/>
-      <c r="BN12" s="41"/>
-      <c r="BO12" s="41"/>
-      <c r="BP12" s="41"/>
-      <c r="BQ12" s="41"/>
-      <c r="BR12" s="39" t="s">
+      <c r="BL12" s="46"/>
+      <c r="BM12" s="46"/>
+      <c r="BN12" s="46"/>
+      <c r="BO12" s="46"/>
+      <c r="BP12" s="46"/>
+      <c r="BQ12" s="46"/>
+      <c r="BR12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="BS12" s="39"/>
-      <c r="BT12" s="39"/>
-      <c r="BU12" s="39"/>
-      <c r="BV12" s="39"/>
-      <c r="BW12" s="39"/>
-      <c r="BX12" s="39"/>
-      <c r="BY12" s="39" t="s">
+      <c r="BS12" s="44"/>
+      <c r="BT12" s="44"/>
+      <c r="BU12" s="44"/>
+      <c r="BV12" s="44"/>
+      <c r="BW12" s="44"/>
+      <c r="BX12" s="44"/>
+      <c r="BY12" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="BZ12" s="39"/>
-      <c r="CA12" s="39"/>
-      <c r="CB12" s="39"/>
-      <c r="CC12" s="39"/>
-      <c r="CD12" s="39"/>
-      <c r="CE12" s="39"/>
-      <c r="CF12" s="39" t="s">
+      <c r="BZ12" s="44"/>
+      <c r="CA12" s="44"/>
+      <c r="CB12" s="44"/>
+      <c r="CC12" s="44"/>
+      <c r="CD12" s="44"/>
+      <c r="CE12" s="44"/>
+      <c r="CF12" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="CG12" s="39"/>
-      <c r="CH12" s="39"/>
-      <c r="CI12" s="39"/>
-      <c r="CJ12" s="39"/>
-      <c r="CK12" s="39"/>
-      <c r="CL12" s="39"/>
-      <c r="CM12" s="39" t="s">
+      <c r="CG12" s="44"/>
+      <c r="CH12" s="44"/>
+      <c r="CI12" s="44"/>
+      <c r="CJ12" s="44"/>
+      <c r="CK12" s="44"/>
+      <c r="CL12" s="44"/>
+      <c r="CM12" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="CN12" s="39"/>
-      <c r="CO12" s="39"/>
-      <c r="CP12" s="39"/>
-      <c r="CQ12" s="39"/>
-      <c r="CR12" s="39"/>
-      <c r="CS12" s="39"/>
-      <c r="CT12" s="39"/>
-      <c r="CU12" s="39"/>
-      <c r="CV12" s="39"/>
-      <c r="CW12" s="39"/>
-      <c r="CX12" s="39"/>
-      <c r="CY12" s="39"/>
-      <c r="CZ12" s="39"/>
-      <c r="DA12" s="39" t="s">
+      <c r="CN12" s="44"/>
+      <c r="CO12" s="44"/>
+      <c r="CP12" s="44"/>
+      <c r="CQ12" s="44"/>
+      <c r="CR12" s="44"/>
+      <c r="CS12" s="44"/>
+      <c r="CT12" s="44"/>
+      <c r="CU12" s="44"/>
+      <c r="CV12" s="44"/>
+      <c r="CW12" s="44"/>
+      <c r="CX12" s="44"/>
+      <c r="CY12" s="44"/>
+      <c r="CZ12" s="44"/>
+      <c r="DA12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="DB12" s="39"/>
-      <c r="DC12" s="39"/>
-      <c r="DD12" s="39"/>
-      <c r="DE12" s="39"/>
-      <c r="DF12" s="39"/>
-      <c r="DG12" s="39"/>
-      <c r="DH12" s="40" t="s">
+      <c r="DB12" s="44"/>
+      <c r="DC12" s="44"/>
+      <c r="DD12" s="44"/>
+      <c r="DE12" s="44"/>
+      <c r="DF12" s="44"/>
+      <c r="DG12" s="44"/>
+      <c r="DH12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="DI12" s="41"/>
-      <c r="DJ12" s="41"/>
-      <c r="DK12" s="41"/>
-      <c r="DL12" s="41"/>
-      <c r="DM12" s="41"/>
-      <c r="DN12" s="42"/>
-      <c r="DO12" s="40" t="s">
+      <c r="DI12" s="46"/>
+      <c r="DJ12" s="46"/>
+      <c r="DK12" s="46"/>
+      <c r="DL12" s="46"/>
+      <c r="DM12" s="46"/>
+      <c r="DN12" s="47"/>
+      <c r="DO12" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="DP12" s="41"/>
-      <c r="DQ12" s="41"/>
-      <c r="DR12" s="41"/>
-      <c r="DS12" s="41"/>
-      <c r="DT12" s="41"/>
-      <c r="DU12" s="42"/>
-      <c r="DV12" s="43" t="s">
+      <c r="DP12" s="46"/>
+      <c r="DQ12" s="46"/>
+      <c r="DR12" s="46"/>
+      <c r="DS12" s="46"/>
+      <c r="DT12" s="46"/>
+      <c r="DU12" s="47"/>
+      <c r="DV12" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="DW12" s="44"/>
-      <c r="DX12" s="44"/>
-      <c r="DY12" s="44"/>
-      <c r="DZ12" s="44"/>
-      <c r="EA12" s="44"/>
-      <c r="EB12" s="45"/>
+      <c r="DW12" s="63"/>
+      <c r="DX12" s="63"/>
+      <c r="DY12" s="63"/>
+      <c r="DZ12" s="63"/>
+      <c r="EA12" s="63"/>
+      <c r="EB12" s="64"/>
       <c r="EC12" s="6"/>
     </row>
     <row r="13" spans="2:135" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3085,7 +3085,7 @@
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
-      <c r="AE20" s="49" t="s">
+      <c r="AE20" s="48" t="s">
         <v>29</v>
       </c>
       <c r="AF20" s="6"/>
@@ -3226,7 +3226,7 @@
       <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
-      <c r="AE21" s="50"/>
+      <c r="AE21" s="49"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
@@ -3365,7 +3365,7 @@
       <c r="AB22" s="6"/>
       <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
-      <c r="AE22" s="50"/>
+      <c r="AE22" s="49"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
@@ -3504,7 +3504,7 @@
       <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
-      <c r="AE23" s="50"/>
+      <c r="AE23" s="49"/>
       <c r="AF23" s="6"/>
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
@@ -3643,7 +3643,7 @@
       <c r="AB24" s="6"/>
       <c r="AC24" s="6"/>
       <c r="AD24" s="6"/>
-      <c r="AE24" s="50"/>
+      <c r="AE24" s="49"/>
       <c r="AF24" s="6"/>
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
@@ -3782,7 +3782,7 @@
       <c r="AB25" s="6"/>
       <c r="AC25" s="6"/>
       <c r="AD25" s="6"/>
-      <c r="AE25" s="50"/>
+      <c r="AE25" s="49"/>
       <c r="AF25" s="6"/>
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
@@ -3921,7 +3921,7 @@
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
-      <c r="AE26" s="50"/>
+      <c r="AE26" s="49"/>
       <c r="AF26" s="6"/>
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
@@ -4060,7 +4060,7 @@
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
       <c r="AD27" s="6"/>
-      <c r="AE27" s="50"/>
+      <c r="AE27" s="49"/>
       <c r="AF27" s="6"/>
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
@@ -4199,7 +4199,7 @@
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
       <c r="AD28" s="6"/>
-      <c r="AE28" s="50"/>
+      <c r="AE28" s="49"/>
       <c r="AF28" s="6"/>
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
@@ -4338,7 +4338,7 @@
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
       <c r="AD29" s="6"/>
-      <c r="AE29" s="50"/>
+      <c r="AE29" s="49"/>
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
@@ -4477,7 +4477,7 @@
       <c r="AB30" s="6"/>
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
-      <c r="AE30" s="50"/>
+      <c r="AE30" s="49"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
@@ -4616,7 +4616,7 @@
       <c r="AB31" s="6"/>
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
-      <c r="AE31" s="50"/>
+      <c r="AE31" s="49"/>
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
@@ -4755,7 +4755,7 @@
       <c r="AB32" s="6"/>
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
-      <c r="AE32" s="50"/>
+      <c r="AE32" s="49"/>
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
@@ -4894,7 +4894,7 @@
       <c r="AB33" s="6"/>
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
-      <c r="AE33" s="50"/>
+      <c r="AE33" s="49"/>
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
@@ -5033,7 +5033,7 @@
       <c r="AB34" s="6"/>
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
-      <c r="AE34" s="50"/>
+      <c r="AE34" s="49"/>
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
@@ -5172,7 +5172,7 @@
       <c r="AB35" s="6"/>
       <c r="AC35" s="6"/>
       <c r="AD35" s="6"/>
-      <c r="AE35" s="50"/>
+      <c r="AE35" s="49"/>
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
@@ -5311,7 +5311,7 @@
       <c r="AB36" s="6"/>
       <c r="AC36" s="6"/>
       <c r="AD36" s="6"/>
-      <c r="AE36" s="50"/>
+      <c r="AE36" s="49"/>
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
@@ -5450,7 +5450,7 @@
       <c r="AB37" s="6"/>
       <c r="AC37" s="6"/>
       <c r="AD37" s="6"/>
-      <c r="AE37" s="50"/>
+      <c r="AE37" s="49"/>
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
@@ -5589,7 +5589,7 @@
       <c r="AB38" s="6"/>
       <c r="AC38" s="6"/>
       <c r="AD38" s="6"/>
-      <c r="AE38" s="50"/>
+      <c r="AE38" s="49"/>
       <c r="AF38" s="6"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
@@ -5728,7 +5728,7 @@
       <c r="AB39" s="6"/>
       <c r="AC39" s="6"/>
       <c r="AD39" s="6"/>
-      <c r="AE39" s="51"/>
+      <c r="AE39" s="50"/>
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
@@ -6534,7 +6534,7 @@
     </row>
     <row r="45" spans="2:133" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
-      <c r="C45" s="62"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="24" t="s">
         <v>78</v>
       </c>
@@ -6544,135 +6544,135 @@
       <c r="F45" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="64"/>
-      <c r="N45" s="64"/>
-      <c r="O45" s="64"/>
-      <c r="P45" s="64"/>
-      <c r="Q45" s="64"/>
-      <c r="R45" s="64"/>
-      <c r="S45" s="64"/>
-      <c r="T45" s="64"/>
-      <c r="U45" s="64"/>
-      <c r="V45" s="64"/>
-      <c r="W45" s="64"/>
-      <c r="X45" s="64"/>
-      <c r="Y45" s="64"/>
-      <c r="Z45" s="64"/>
-      <c r="AA45" s="64"/>
-      <c r="AB45" s="64"/>
-      <c r="AC45" s="64"/>
-      <c r="AD45" s="64"/>
-      <c r="AE45" s="64"/>
-      <c r="AF45" s="64"/>
-      <c r="AG45" s="64"/>
-      <c r="AH45" s="64"/>
-      <c r="AI45" s="64"/>
-      <c r="AJ45" s="64"/>
-      <c r="AK45" s="64"/>
-      <c r="AL45" s="64"/>
-      <c r="AM45" s="64"/>
-      <c r="AN45" s="64"/>
-      <c r="AO45" s="64"/>
-      <c r="AP45" s="64"/>
-      <c r="AQ45" s="64"/>
-      <c r="AR45" s="64"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
+      <c r="P45" s="41"/>
+      <c r="Q45" s="41"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="41"/>
+      <c r="T45" s="41"/>
+      <c r="U45" s="41"/>
+      <c r="V45" s="41"/>
+      <c r="W45" s="41"/>
+      <c r="X45" s="41"/>
+      <c r="Y45" s="41"/>
+      <c r="Z45" s="41"/>
+      <c r="AA45" s="41"/>
+      <c r="AB45" s="41"/>
+      <c r="AC45" s="41"/>
+      <c r="AD45" s="41"/>
+      <c r="AE45" s="41"/>
+      <c r="AF45" s="41"/>
+      <c r="AG45" s="41"/>
+      <c r="AH45" s="41"/>
+      <c r="AI45" s="41"/>
+      <c r="AJ45" s="41"/>
+      <c r="AK45" s="41"/>
+      <c r="AL45" s="41"/>
+      <c r="AM45" s="41"/>
+      <c r="AN45" s="41"/>
+      <c r="AO45" s="41"/>
+      <c r="AP45" s="41"/>
+      <c r="AQ45" s="41"/>
+      <c r="AR45" s="41"/>
       <c r="AS45" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AT45" s="64"/>
-      <c r="AU45" s="64"/>
-      <c r="AV45" s="64"/>
-      <c r="AW45" s="64"/>
-      <c r="AX45" s="64"/>
-      <c r="AY45" s="64"/>
-      <c r="AZ45" s="64"/>
-      <c r="BA45" s="64"/>
-      <c r="BB45" s="64"/>
-      <c r="BC45" s="64"/>
-      <c r="BD45" s="64"/>
-      <c r="BE45" s="64"/>
-      <c r="BF45" s="64"/>
-      <c r="BG45" s="64"/>
-      <c r="BH45" s="64"/>
-      <c r="BI45" s="64"/>
-      <c r="BJ45" s="64"/>
-      <c r="BK45" s="64"/>
-      <c r="BL45" s="64"/>
-      <c r="BM45" s="64"/>
-      <c r="BN45" s="64"/>
-      <c r="BO45" s="64"/>
-      <c r="BP45" s="64"/>
-      <c r="BQ45" s="64"/>
-      <c r="BR45" s="64"/>
-      <c r="BS45" s="64"/>
-      <c r="BT45" s="64"/>
-      <c r="BU45" s="64"/>
-      <c r="BV45" s="64"/>
-      <c r="BW45" s="64"/>
-      <c r="BX45" s="64"/>
-      <c r="BY45" s="64"/>
-      <c r="BZ45" s="64"/>
-      <c r="CA45" s="64"/>
-      <c r="CB45" s="64"/>
-      <c r="CC45" s="64"/>
-      <c r="CD45" s="64"/>
-      <c r="CE45" s="64"/>
-      <c r="CF45" s="64"/>
-      <c r="CG45" s="64"/>
-      <c r="CH45" s="64"/>
-      <c r="CI45" s="64"/>
-      <c r="CJ45" s="64"/>
-      <c r="CK45" s="64"/>
-      <c r="CL45" s="64"/>
-      <c r="CM45" s="64"/>
-      <c r="CN45" s="64"/>
-      <c r="CO45" s="64"/>
-      <c r="CP45" s="64"/>
-      <c r="CQ45" s="64"/>
-      <c r="CR45" s="64"/>
-      <c r="CS45" s="64"/>
-      <c r="CT45" s="64"/>
-      <c r="CU45" s="64"/>
-      <c r="CV45" s="64"/>
-      <c r="CW45" s="64"/>
-      <c r="CX45" s="64"/>
-      <c r="CY45" s="64"/>
-      <c r="CZ45" s="64"/>
-      <c r="DA45" s="64"/>
-      <c r="DB45" s="64"/>
-      <c r="DC45" s="64"/>
-      <c r="DD45" s="64"/>
-      <c r="DE45" s="64"/>
-      <c r="DF45" s="64"/>
-      <c r="DG45" s="64"/>
-      <c r="DH45" s="64"/>
-      <c r="DI45" s="64"/>
-      <c r="DJ45" s="64"/>
-      <c r="DK45" s="64"/>
-      <c r="DL45" s="64"/>
-      <c r="DM45" s="64"/>
-      <c r="DN45" s="64"/>
-      <c r="DO45" s="64"/>
-      <c r="DP45" s="64"/>
-      <c r="DQ45" s="64"/>
-      <c r="DR45" s="64"/>
-      <c r="DS45" s="64"/>
-      <c r="DT45" s="64"/>
-      <c r="DU45" s="64"/>
-      <c r="DV45" s="64"/>
-      <c r="DW45" s="64"/>
-      <c r="DX45" s="64"/>
-      <c r="DY45" s="64"/>
-      <c r="DZ45" s="64"/>
-      <c r="EA45" s="64"/>
-      <c r="EB45" s="64"/>
-      <c r="EC45" s="64"/>
+      <c r="AT45" s="41"/>
+      <c r="AU45" s="41"/>
+      <c r="AV45" s="41"/>
+      <c r="AW45" s="41"/>
+      <c r="AX45" s="41"/>
+      <c r="AY45" s="41"/>
+      <c r="AZ45" s="41"/>
+      <c r="BA45" s="41"/>
+      <c r="BB45" s="41"/>
+      <c r="BC45" s="41"/>
+      <c r="BD45" s="41"/>
+      <c r="BE45" s="41"/>
+      <c r="BF45" s="41"/>
+      <c r="BG45" s="41"/>
+      <c r="BH45" s="41"/>
+      <c r="BI45" s="41"/>
+      <c r="BJ45" s="41"/>
+      <c r="BK45" s="41"/>
+      <c r="BL45" s="41"/>
+      <c r="BM45" s="41"/>
+      <c r="BN45" s="41"/>
+      <c r="BO45" s="41"/>
+      <c r="BP45" s="41"/>
+      <c r="BQ45" s="41"/>
+      <c r="BR45" s="41"/>
+      <c r="BS45" s="41"/>
+      <c r="BT45" s="41"/>
+      <c r="BU45" s="41"/>
+      <c r="BV45" s="41"/>
+      <c r="BW45" s="41"/>
+      <c r="BX45" s="41"/>
+      <c r="BY45" s="41"/>
+      <c r="BZ45" s="41"/>
+      <c r="CA45" s="41"/>
+      <c r="CB45" s="41"/>
+      <c r="CC45" s="41"/>
+      <c r="CD45" s="41"/>
+      <c r="CE45" s="41"/>
+      <c r="CF45" s="41"/>
+      <c r="CG45" s="41"/>
+      <c r="CH45" s="41"/>
+      <c r="CI45" s="41"/>
+      <c r="CJ45" s="41"/>
+      <c r="CK45" s="41"/>
+      <c r="CL45" s="41"/>
+      <c r="CM45" s="41"/>
+      <c r="CN45" s="41"/>
+      <c r="CO45" s="41"/>
+      <c r="CP45" s="41"/>
+      <c r="CQ45" s="41"/>
+      <c r="CR45" s="41"/>
+      <c r="CS45" s="41"/>
+      <c r="CT45" s="41"/>
+      <c r="CU45" s="41"/>
+      <c r="CV45" s="41"/>
+      <c r="CW45" s="41"/>
+      <c r="CX45" s="41"/>
+      <c r="CY45" s="41"/>
+      <c r="CZ45" s="41"/>
+      <c r="DA45" s="41"/>
+      <c r="DB45" s="41"/>
+      <c r="DC45" s="41"/>
+      <c r="DD45" s="41"/>
+      <c r="DE45" s="41"/>
+      <c r="DF45" s="41"/>
+      <c r="DG45" s="41"/>
+      <c r="DH45" s="41"/>
+      <c r="DI45" s="41"/>
+      <c r="DJ45" s="41"/>
+      <c r="DK45" s="41"/>
+      <c r="DL45" s="41"/>
+      <c r="DM45" s="41"/>
+      <c r="DN45" s="41"/>
+      <c r="DO45" s="41"/>
+      <c r="DP45" s="41"/>
+      <c r="DQ45" s="41"/>
+      <c r="DR45" s="41"/>
+      <c r="DS45" s="41"/>
+      <c r="DT45" s="41"/>
+      <c r="DU45" s="41"/>
+      <c r="DV45" s="41"/>
+      <c r="DW45" s="41"/>
+      <c r="DX45" s="41"/>
+      <c r="DY45" s="41"/>
+      <c r="DZ45" s="41"/>
+      <c r="EA45" s="41"/>
+      <c r="EB45" s="41"/>
+      <c r="EC45" s="41"/>
     </row>
     <row r="46" spans="2:133" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="17"/>
@@ -9471,27 +9471,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="AN10:BQ11"/>
-    <mergeCell ref="BR12:BX12"/>
-    <mergeCell ref="AP12:AV12"/>
-    <mergeCell ref="AW12:BC12"/>
-    <mergeCell ref="AE20:AE39"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="G10:AM11"/>
-    <mergeCell ref="AI12:AM12"/>
-    <mergeCell ref="BD12:BJ12"/>
-    <mergeCell ref="BK12:BQ12"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="N12:T12"/>
-    <mergeCell ref="U12:AA12"/>
-    <mergeCell ref="AB12:AH12"/>
-    <mergeCell ref="AN12:AO12"/>
     <mergeCell ref="DA12:DG12"/>
     <mergeCell ref="DH12:DN12"/>
     <mergeCell ref="DO12:DU12"/>
@@ -9503,8 +9482,30 @@
     <mergeCell ref="CM12:CS12"/>
     <mergeCell ref="CT12:CV12"/>
     <mergeCell ref="CW12:CZ12"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="AN10:BQ11"/>
+    <mergeCell ref="BR12:BX12"/>
+    <mergeCell ref="AP12:AV12"/>
+    <mergeCell ref="AW12:BC12"/>
+    <mergeCell ref="AE20:AE39"/>
+    <mergeCell ref="G10:AM11"/>
+    <mergeCell ref="AI12:AM12"/>
+    <mergeCell ref="BD12:BJ12"/>
+    <mergeCell ref="BK12:BQ12"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="N12:T12"/>
+    <mergeCell ref="U12:AA12"/>
+    <mergeCell ref="AB12:AH12"/>
+    <mergeCell ref="AN12:AO12"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>